<commit_message>
modified some figures and added a table
</commit_message>
<xml_diff>
--- a/data/2020-07-24_AgNP-ELA-lakes_fish-excretion.xlsx
+++ b/data/2020-07-24_AgNP-ELA-lakes_fish-excretion.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="27" documentId="8_{CE3E8D6E-5903-41F8-A84F-7FD18A12D88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64A9B145-CB35-4D8C-A758-60E998DFD4E2}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="889" firstSheet="4" activeTab="14" xr2:uid="{33E7FBB4-830F-460A-98F2-8A56863560C3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="889" firstSheet="1" activeTab="3" xr2:uid="{33E7FBB4-830F-460A-98F2-8A56863560C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="3" r:id="rId1"/>
@@ -4894,14 +4894,10 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4939,7 +4935,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5045,7 +5041,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5187,7 +5183,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5197,7 +5193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A0575C-80C8-4FDD-B941-7E4C95A45360}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -5212,7 +5208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E1956D-EFBD-4593-BE1B-2E5DF391B8BF}">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M2" activeCellId="1" sqref="B2:B52 M2:M52"/>
     </sheetView>
   </sheetViews>
@@ -11860,11 +11856,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FAD8F5-A8BD-45AA-BE9B-3586B79614F6}">
   <dimension ref="A1:AK151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D131" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="S44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R142" sqref="R142"/>
+      <selection pane="bottomRight" activeCell="AA76" sqref="AA72:AA76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -29525,8 +29521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E2F93D-1A32-447F-B047-7B2FE78CD02E}">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30618,7 +30614,7 @@
   <dimension ref="A1:M244"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
@@ -39206,7 +39202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C37933-0603-43DD-B7AC-E2616142588C}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -40292,7 +40288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C8F2B9-D7DD-4C2B-95C0-6DBE614B7468}">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>

</xml_diff>